<commit_message>
Updated via the Open Science Framework
</commit_message>
<xml_diff>
--- a/Codice/Codice_Polarity_final/Results_FT.xlsx
+++ b/Codice/Codice_Polarity_final/Results_FT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fossati\Desktop\Tesi\Codice\Codice_FineTuningBERT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3BC37A-B954-4E22-976F-C182184F50B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03303E66-3973-48C5-9914-DC12B0A224CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{1A932559-5FD6-4256-BF9F-E74E86ABA7F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="189">
   <si>
     <t>Accuracy</t>
   </si>
@@ -575,9 +575,6 @@
     <t>0.98</t>
   </si>
   <si>
-    <t>Benc_IT</t>
-  </si>
-  <si>
     <t>Benc_EN1</t>
   </si>
   <si>
@@ -593,17 +590,26 @@
     <t>0.48</t>
   </si>
   <si>
-    <t>BencEN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BencEN2</t>
+    <t>SST_help</t>
+  </si>
+  <si>
+    <t>Bench_SST</t>
+  </si>
+  <si>
+    <t>XLMR</t>
+  </si>
+  <si>
+    <t>mBERT</t>
+  </si>
+  <si>
+    <t>0.33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,8 +623,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,8 +693,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -824,11 +844,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -896,6 +927,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1212,15 +1251,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E444A59-07F3-4DC8-A33F-5BD860DB2BB6}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1234,25 +1273,21 @@
         <v>3</v>
       </c>
       <c r="F1" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1268,11 +1303,17 @@
       <c r="E3" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1290,9 +1331,8 @@
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1310,9 +1350,8 @@
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1330,675 +1369,613 @@
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>40</v>
+        <v>188</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>41</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>47</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>31</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>50</v>
-      </c>
       <c r="D25" s="26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>34</v>
       </c>
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F28" s="25"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>66</v>
+        <v>22</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>151</v>
+        <v>24</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="26" t="s">
-        <v>40</v>
-      </c>
       <c r="E33" s="26" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>39</v>
+        <v>26</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>66</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>154</v>
+        <v>27</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C38" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H38" s="35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>41</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>163</v>
+        <v>43</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>48</v>
       </c>
       <c r="E41" s="26" t="s">
         <v>67</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D43" s="26" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B44" s="26" t="s">
         <v>51</v>
@@ -2007,149 +1984,139 @@
         <v>53</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>46</v>
+        <v>137</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="26" t="s">
         <v>49</v>
       </c>
+      <c r="C46" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>163</v>
+      </c>
       <c r="E46" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="29" t="s">
-        <v>66</v>
+      <c r="E48" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="H48" s="26" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="G48" s="40" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="30" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>53</v>
+        <v>137</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B51" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D51" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E51" s="32" t="s">
-        <v>178</v>
+      <c r="E51" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
     </row>
     <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="27"/>
@@ -2158,93 +2125,175 @@
       <c r="E52" s="27"/>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="F53" s="35" t="s">
-        <v>38</v>
+        <v>176</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="30" t="s">
         <v>67</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E54" s="26" t="s">
-        <v>163</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
+      <c r="H54" s="37"/>
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" s="26" t="s">
-        <v>41</v>
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="33" t="s">
-        <v>53</v>
+        <v>171</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E56" s="32" t="s">
         <v>178</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+    </row>
+    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2257,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB2F3DA-6234-48B4-AD4B-4A90FAE49373}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,10 +2321,10 @@
         <v>98</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2979,10 +3028,10 @@
         <v>168</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -3012,10 +3061,10 @@
         <v>171</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>